<commit_message>
test1 passed for s_simu(exc_st3 , tg , pss)
</commit_message>
<xml_diff>
--- a/test_functions/test_exc3_pss_tg/Test/output_exc_st3.xlsx
+++ b/test_functions/test_exc3_pss_tg/Test/output_exc_st3.xlsx
@@ -178,7 +178,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="2" width="15.77"/>
@@ -274,7 +274,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -321,7 +321,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -368,7 +368,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -412,10 +412,10 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -462,7 +462,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -509,7 +509,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -556,7 +556,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="15.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.66"/>
@@ -626,7 +626,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>
@@ -673,7 +673,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="15.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="42.22"/>
@@ -743,7 +743,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="15.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="42.22"/>
@@ -813,7 +813,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="15.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="42.22"/>
@@ -861,10 +861,10 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.78125" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7734375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="15.77"/>
   </cols>

</xml_diff>